<commit_message>
Cuaderno decimo tema 4
Cuaderno décimo tema 4
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion02/Escaleta_MA_11_02_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion02/Escaleta_MA_11_02_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado11\guion02\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25598" windowHeight="14723"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -18,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -380,9 +375,6 @@
   </si>
   <si>
     <t>Practica las operaciones entre funciones</t>
-  </si>
-  <si>
-    <t>Actividad para identificar la función inversa a la función trigonométrica dada</t>
   </si>
   <si>
     <t>Competencias</t>
@@ -904,6 +896,9 @@
   </si>
   <si>
     <t>Recurso M101A-04</t>
+  </si>
+  <si>
+    <t>Actividad para identificar la función inversa a la función dada</t>
   </si>
 </sst>
 </file>
@@ -1271,12 +1266,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1293,51 +1333,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1430,7 +1425,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1465,7 +1460,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1676,127 +1671,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T21" sqref="T21"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.46484375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.46484375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="22.1328125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="16" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="31.1328125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="16" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="25.46484375" style="24" customWidth="1"/>
-    <col min="7" max="7" width="40.796875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="9.46484375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="25.5" style="24" customWidth="1"/>
+    <col min="7" max="7" width="40.83203125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="24" customWidth="1"/>
     <col min="9" max="9" width="11" style="24" customWidth="1"/>
-    <col min="10" max="10" width="17.796875" style="40" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="40" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" style="16" customWidth="1"/>
-    <col min="12" max="12" width="17.46484375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="16" customWidth="1"/>
     <col min="13" max="14" width="9.33203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="37.796875" style="24" customWidth="1"/>
-    <col min="16" max="16" width="16.46484375" style="24" customWidth="1"/>
+    <col min="15" max="15" width="37.83203125" style="24" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="24" customWidth="1"/>
     <col min="17" max="17" width="19.6640625" style="36" customWidth="1"/>
-    <col min="18" max="18" width="21.46484375" style="37" customWidth="1"/>
-    <col min="19" max="19" width="20.796875" style="39" customWidth="1"/>
-    <col min="20" max="20" width="23.796875" style="37" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.796875" style="37" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="11.46484375" style="16"/>
+    <col min="18" max="18" width="21.5" style="37" customWidth="1"/>
+    <col min="19" max="19" width="20.83203125" style="39" customWidth="1"/>
+    <col min="20" max="20" width="23.83203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.83203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.5" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:21" s="17" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="O1" s="41" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="43" t="s">
+      <c r="S1" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="T1" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="54"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="56"/>
+    <row r="2" spans="1:21" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="44"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="59"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" thickTop="1">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
@@ -1812,7 +1807,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="4"/>
       <c r="G3" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H3" s="7">
         <v>1</v>
@@ -1830,11 +1825,11 @@
         <v>5</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>19</v>
@@ -1843,19 +1838,19 @@
         <v>6</v>
       </c>
       <c r="R3" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="T3" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="U3" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="T3" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="U3" s="33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
@@ -1880,7 +1875,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>20</v>
@@ -1900,19 +1895,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S4" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="T4" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="T4" s="35" t="s">
+      <c r="U4" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="U4" s="33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
@@ -1928,7 +1923,7 @@
       <c r="E5" s="19"/>
       <c r="F5" s="5"/>
       <c r="G5" s="30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" s="8">
         <v>3</v>
@@ -1937,7 +1932,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>20</v>
@@ -1947,10 +1942,10 @@
       </c>
       <c r="M5" s="23"/>
       <c r="N5" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>19</v>
@@ -1959,19 +1954,19 @@
         <v>6</v>
       </c>
       <c r="R5" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S5" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S5" s="38" t="s">
+      <c r="T5" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="T5" s="35" t="s">
+      <c r="U5" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="U5" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -1987,7 +1982,7 @@
       <c r="E6" s="19"/>
       <c r="F6" s="5"/>
       <c r="G6" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H6" s="8">
         <v>4</v>
@@ -1996,7 +1991,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>20</v>
@@ -2006,10 +2001,10 @@
       </c>
       <c r="M6" s="23"/>
       <c r="N6" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="O6" s="26" t="s">
         <v>164</v>
-      </c>
-      <c r="O6" s="26" t="s">
-        <v>165</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>20</v>
@@ -2018,19 +2013,19 @@
         <v>6</v>
       </c>
       <c r="R6" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S6" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S6" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T6" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U6" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
@@ -2057,7 +2052,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>20</v>
@@ -2067,10 +2062,10 @@
       </c>
       <c r="M7" s="23"/>
       <c r="N7" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O7" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>19</v>
@@ -2079,19 +2074,19 @@
         <v>6</v>
       </c>
       <c r="R7" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S7" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S7" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T7" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="U7" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -2102,12 +2097,12 @@
         <v>86</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="5"/>
       <c r="G8" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" s="8">
         <v>6</v>
@@ -2116,7 +2111,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>20</v>
@@ -2125,11 +2120,11 @@
         <v>5</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>19</v>
@@ -2138,19 +2133,19 @@
         <v>6</v>
       </c>
       <c r="R8" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="S8" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="S8" s="38" t="s">
+      <c r="T8" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="U8" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="T8" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="U8" s="33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -2161,12 +2156,12 @@
         <v>86</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="5"/>
       <c r="G9" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H9" s="8">
         <v>7</v>
@@ -2175,7 +2170,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>20</v>
@@ -2185,10 +2180,10 @@
       </c>
       <c r="M9" s="23"/>
       <c r="N9" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>19</v>
@@ -2197,19 +2192,19 @@
         <v>6</v>
       </c>
       <c r="R9" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S9" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S9" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T9" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U9" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>15</v>
       </c>
@@ -2220,12 +2215,12 @@
         <v>86</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="5"/>
       <c r="G10" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H10" s="8">
         <v>8</v>
@@ -2234,7 +2229,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>20</v>
@@ -2244,10 +2239,10 @@
       </c>
       <c r="M10" s="23"/>
       <c r="N10" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="O10" s="26" t="s">
         <v>169</v>
-      </c>
-      <c r="O10" s="26" t="s">
-        <v>170</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>19</v>
@@ -2256,19 +2251,19 @@
         <v>6</v>
       </c>
       <c r="R10" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S10" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S10" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T10" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="U10" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>15</v>
       </c>
@@ -2279,12 +2274,12 @@
         <v>86</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="5"/>
       <c r="G11" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H11" s="7">
         <v>9</v>
@@ -2293,7 +2288,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K11" s="21" t="s">
         <v>20</v>
@@ -2303,10 +2298,10 @@
       </c>
       <c r="M11" s="23"/>
       <c r="N11" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="O11" s="26" t="s">
         <v>200</v>
-      </c>
-      <c r="O11" s="26" t="s">
-        <v>201</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>19</v>
@@ -2315,19 +2310,19 @@
         <v>6</v>
       </c>
       <c r="R11" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S11" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S11" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T11" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U11" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
@@ -2338,14 +2333,14 @@
         <v>86</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>90</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H12" s="8">
         <v>10</v>
@@ -2354,7 +2349,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>20</v>
@@ -2364,10 +2359,10 @@
       </c>
       <c r="M12" s="23"/>
       <c r="N12" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O12" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>19</v>
@@ -2376,19 +2371,19 @@
         <v>6</v>
       </c>
       <c r="R12" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S12" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S12" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T12" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U12" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2399,12 +2394,12 @@
         <v>86</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="5"/>
       <c r="G13" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H13" s="8">
         <v>11</v>
@@ -2413,7 +2408,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K13" s="21" t="s">
         <v>20</v>
@@ -2422,11 +2417,11 @@
         <v>5</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N13" s="23"/>
       <c r="O13" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>19</v>
@@ -2435,19 +2430,19 @@
         <v>6</v>
       </c>
       <c r="R13" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="S13" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="S13" s="38" t="s">
+      <c r="T13" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="U13" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="T13" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="U13" s="33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
@@ -2458,12 +2453,12 @@
         <v>86</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="5"/>
       <c r="G14" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H14" s="8">
         <v>12</v>
@@ -2472,7 +2467,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>20</v>
@@ -2482,10 +2477,10 @@
       </c>
       <c r="M14" s="23"/>
       <c r="N14" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O14" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>19</v>
@@ -2494,19 +2489,19 @@
         <v>6</v>
       </c>
       <c r="R14" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S14" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S14" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T14" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U14" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
@@ -2517,12 +2512,12 @@
         <v>86</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="5"/>
       <c r="G15" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H15" s="8">
         <v>13</v>
@@ -2531,7 +2526,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>20</v>
@@ -2541,10 +2536,10 @@
       </c>
       <c r="M15" s="23"/>
       <c r="N15" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O15" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>20</v>
@@ -2553,19 +2548,19 @@
         <v>6</v>
       </c>
       <c r="R15" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S15" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S15" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T15" s="35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U15" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1">
       <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
@@ -2576,12 +2571,12 @@
         <v>86</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="5"/>
       <c r="G16" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H16" s="7">
         <v>14</v>
@@ -2590,7 +2585,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K16" s="21" t="s">
         <v>20</v>
@@ -2600,10 +2595,10 @@
       </c>
       <c r="M16" s="23"/>
       <c r="N16" s="23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O16" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>19</v>
@@ -2612,19 +2607,19 @@
         <v>6</v>
       </c>
       <c r="R16" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S16" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S16" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T16" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="U16" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
@@ -2635,14 +2630,14 @@
         <v>86</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>90</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H17" s="8">
         <v>15</v>
@@ -2651,7 +2646,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>20</v>
@@ -2661,10 +2656,10 @@
       </c>
       <c r="M17" s="23"/>
       <c r="N17" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="O17" s="26" t="s">
         <v>173</v>
-      </c>
-      <c r="O17" s="26" t="s">
-        <v>174</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>19</v>
@@ -2673,19 +2668,19 @@
         <v>6</v>
       </c>
       <c r="R17" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S17" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S17" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T17" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U17" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
@@ -2696,12 +2691,12 @@
         <v>86</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="5"/>
       <c r="G18" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H18" s="8">
         <v>16</v>
@@ -2710,7 +2705,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>20</v>
@@ -2720,10 +2715,10 @@
       </c>
       <c r="M18" s="23"/>
       <c r="N18" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O18" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>19</v>
@@ -2732,19 +2727,19 @@
         <v>6</v>
       </c>
       <c r="R18" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S18" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S18" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T18" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U18" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15" customHeight="1">
       <c r="A19" s="9" t="s">
         <v>15</v>
       </c>
@@ -2755,12 +2750,12 @@
         <v>86</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="5"/>
       <c r="G19" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H19" s="8">
         <v>17</v>
@@ -2769,7 +2764,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>96</v>
+        <v>216</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>20</v>
@@ -2779,10 +2774,10 @@
       </c>
       <c r="M19" s="23"/>
       <c r="N19" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>19</v>
@@ -2791,19 +2786,19 @@
         <v>6</v>
       </c>
       <c r="R19" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S19" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S19" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T19" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U19" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>15</v>
       </c>
@@ -2814,12 +2809,12 @@
         <v>86</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="5"/>
       <c r="G20" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H20" s="8">
         <v>18</v>
@@ -2828,7 +2823,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>20</v>
@@ -2838,10 +2833,10 @@
       </c>
       <c r="M20" s="23"/>
       <c r="N20" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O20" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>19</v>
@@ -2850,19 +2845,19 @@
         <v>6</v>
       </c>
       <c r="R20" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S20" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S20" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T20" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U20" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>15</v>
       </c>
@@ -2873,12 +2868,12 @@
         <v>86</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="5"/>
       <c r="G21" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H21" s="8">
         <v>19</v>
@@ -2896,7 +2891,7 @@
         <v>5</v>
       </c>
       <c r="M21" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N21" s="23"/>
       <c r="O21" s="26" t="s">
@@ -2909,19 +2904,19 @@
         <v>6</v>
       </c>
       <c r="R21" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="S21" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="S21" s="38" t="s">
+      <c r="T21" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="U21" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="T21" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="U21" s="33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:21" ht="15" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>15</v>
       </c>
@@ -2932,7 +2927,7 @@
         <v>86</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="5"/>
@@ -2946,7 +2941,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>20</v>
@@ -2956,10 +2951,10 @@
       </c>
       <c r="M22" s="23"/>
       <c r="N22" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>19</v>
@@ -2968,19 +2963,19 @@
         <v>6</v>
       </c>
       <c r="R22" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S22" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S22" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T22" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U22" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15" customHeight="1">
       <c r="A23" s="9" t="s">
         <v>15</v>
       </c>
@@ -2991,12 +2986,12 @@
         <v>86</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="5"/>
       <c r="G23" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H23" s="8">
         <v>21</v>
@@ -3005,7 +3000,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>20</v>
@@ -3015,10 +3010,10 @@
       </c>
       <c r="M23" s="23"/>
       <c r="N23" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="O23" s="26" t="s">
         <v>189</v>
-      </c>
-      <c r="O23" s="26" t="s">
-        <v>190</v>
       </c>
       <c r="P23" s="6" t="s">
         <v>19</v>
@@ -3027,19 +3022,19 @@
         <v>6</v>
       </c>
       <c r="R23" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S23" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S23" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T23" s="35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U23" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15" customHeight="1">
       <c r="A24" s="9" t="s">
         <v>15</v>
       </c>
@@ -3050,14 +3045,14 @@
         <v>86</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>90</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H24" s="8">
         <v>22</v>
@@ -3066,7 +3061,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>20</v>
@@ -3076,10 +3071,10 @@
       </c>
       <c r="M24" s="23"/>
       <c r="N24" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O24" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P24" s="6" t="s">
         <v>19</v>
@@ -3088,19 +3083,19 @@
         <v>6</v>
       </c>
       <c r="R24" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S24" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S24" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T24" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U24" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15" customHeight="1">
       <c r="A25" s="9" t="s">
         <v>15</v>
       </c>
@@ -3111,14 +3106,14 @@
         <v>86</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>90</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H25" s="8">
         <v>23</v>
@@ -3127,7 +3122,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K25" s="21" t="s">
         <v>20</v>
@@ -3137,10 +3132,10 @@
       </c>
       <c r="M25" s="23"/>
       <c r="N25" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O25" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>20</v>
@@ -3149,19 +3144,19 @@
         <v>6</v>
       </c>
       <c r="R25" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S25" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S25" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T25" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U25" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15" customHeight="1">
       <c r="A26" s="9" t="s">
         <v>15</v>
       </c>
@@ -3172,12 +3167,12 @@
         <v>86</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="5"/>
       <c r="G26" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H26" s="8">
         <v>24</v>
@@ -3186,7 +3181,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K26" s="21" t="s">
         <v>20</v>
@@ -3196,10 +3191,10 @@
       </c>
       <c r="M26" s="23"/>
       <c r="N26" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O26" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P26" s="6" t="s">
         <v>19</v>
@@ -3208,19 +3203,19 @@
         <v>6</v>
       </c>
       <c r="R26" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S26" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S26" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T26" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U26" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="15" customHeight="1">
       <c r="A27" s="9" t="s">
         <v>15</v>
       </c>
@@ -3231,12 +3226,12 @@
         <v>86</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="5"/>
       <c r="G27" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H27" s="7">
         <v>25</v>
@@ -3245,7 +3240,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>20</v>
@@ -3255,10 +3250,10 @@
       </c>
       <c r="M27" s="23"/>
       <c r="N27" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O27" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>19</v>
@@ -3267,19 +3262,19 @@
         <v>6</v>
       </c>
       <c r="R27" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S27" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S27" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T27" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U27" s="33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="15" customHeight="1">
       <c r="A28" s="9" t="s">
         <v>15</v>
       </c>
@@ -3290,7 +3285,7 @@
         <v>86</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="5"/>
@@ -3304,7 +3299,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>20</v>
@@ -3324,7 +3319,7 @@
       <c r="T28" s="35"/>
       <c r="U28" s="33"/>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21" ht="15" customHeight="1">
       <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
@@ -3335,12 +3330,12 @@
         <v>86</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="5"/>
       <c r="G29" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H29" s="8">
         <v>27</v>
@@ -3349,7 +3344,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K29" s="21" t="s">
         <v>20</v>
@@ -3359,10 +3354,10 @@
       </c>
       <c r="M29" s="23"/>
       <c r="N29" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O29" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P29" s="6" t="s">
         <v>20</v>
@@ -3371,16 +3366,16 @@
         <v>6</v>
       </c>
       <c r="R29" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="S29" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="S29" s="38" t="s">
-        <v>109</v>
-      </c>
       <c r="T29" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U29" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3388,6 +3383,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3402,12 +3403,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3460,27 +3455,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.46484375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.46484375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.46484375" style="1"/>
+    <col min="13" max="13" width="11.5" style="1"/>
     <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.46484375" style="1"/>
+    <col min="15" max="15" width="69.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3497,7 +3492,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -3521,7 +3516,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -3540,7 +3535,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -3559,7 +3554,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -3575,7 +3570,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -3592,7 +3587,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3609,7 +3604,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3624,7 +3619,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -3639,7 +3634,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3654,7 +3649,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3669,7 +3664,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3684,7 +3679,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -3699,7 +3694,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -3714,7 +3709,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -3729,7 +3724,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -3744,7 +3739,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -3758,7 +3753,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -3772,7 +3767,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -3786,7 +3781,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -3800,7 +3795,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -3815,7 +3810,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -3830,7 +3825,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3845,7 +3840,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -3860,7 +3855,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -3875,7 +3870,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3890,7 +3885,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3905,7 +3900,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3920,7 +3915,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3935,7 +3930,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -3950,7 +3945,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -3965,7 +3960,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -3980,7 +3975,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -3995,7 +3990,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -4010,7 +4005,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -4025,7 +4020,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -4040,7 +4035,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -4055,7 +4050,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -4070,7 +4065,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -4085,7 +4080,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -4100,7 +4095,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -4115,7 +4110,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -4130,7 +4125,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -4145,7 +4140,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -4160,7 +4155,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -4175,7 +4170,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -4190,7 +4185,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -4205,7 +4200,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -4220,7 +4215,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -4232,7 +4227,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -4244,7 +4239,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -4257,7 +4252,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -4270,7 +4265,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -4283,7 +4278,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -4296,7 +4291,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -4309,7 +4304,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -4322,7 +4317,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -4335,7 +4330,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -4348,7 +4343,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -4361,7 +4356,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -4374,7 +4369,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -4387,7 +4382,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -4400,7 +4395,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -4413,7 +4408,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -4426,7 +4421,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -4439,7 +4434,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -4452,7 +4447,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -4465,7 +4460,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -4478,7 +4473,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -4491,7 +4486,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -4504,7 +4499,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -4518,7 +4513,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -4532,7 +4527,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -4546,7 +4541,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -4560,7 +4555,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -4574,7 +4569,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -4588,7 +4583,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -4602,7 +4597,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -4616,7 +4611,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -4630,7 +4625,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4644,7 +4639,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -4658,7 +4653,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -4672,7 +4667,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -4686,7 +4681,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -4700,7 +4695,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -4714,7 +4709,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -4728,7 +4723,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -4742,7 +4737,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -4756,7 +4751,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -4770,7 +4765,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4784,7 +4779,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4798,7 +4793,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4812,7 +4807,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -4826,7 +4821,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -4840,7 +4835,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4854,7 +4849,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -4868,7 +4863,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -4882,7 +4877,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -4896,7 +4891,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -4910,7 +4905,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -4924,7 +4919,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -4938,7 +4933,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4952,7 +4947,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -4966,7 +4961,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -4980,7 +4975,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4994,7 +4989,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -5008,7 +5003,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -5022,7 +5017,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -5036,7 +5031,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -5050,7 +5045,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -5064,7 +5059,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -5078,7 +5073,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -5092,7 +5087,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -5106,7 +5101,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -5120,7 +5115,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -5134,7 +5129,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -5148,7 +5143,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -5162,7 +5157,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -5176,7 +5171,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -5190,7 +5185,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -5204,7 +5199,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -5218,7 +5213,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -5232,7 +5227,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -5246,7 +5241,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -5260,7 +5255,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -5274,7 +5269,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -5288,7 +5283,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -5302,7 +5297,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -5316,7 +5311,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -5330,7 +5325,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -5344,7 +5339,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -5358,7 +5353,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -5372,7 +5367,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>

</xml_diff>